<commit_message>
work on individual model
-started implementation of individual vehicles
</commit_message>
<xml_diff>
--- a/vehicleplan.xlsx
+++ b/vehicleplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadvi\Documents\GitHub\V2G-optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEE0401-3069-4B7F-9750-697AA1F6F140}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7D3A95-268E-4203-8340-354AFD2D3005}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="3990" windowWidth="21600" windowHeight="12735" xr2:uid="{6C18CA4E-8E16-4EFD-98A4-AD0010013D9F}"/>
+    <workbookView xWindow="5760" yWindow="1500" windowWidth="21600" windowHeight="13155" xr2:uid="{6C18CA4E-8E16-4EFD-98A4-AD0010013D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Battery capacity in kWh</t>
   </si>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B5C34C-4A0A-4DE6-8BE8-9894332D3D15}">
   <dimension ref="A2:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="T72" sqref="T72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>0.5</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>0.55000000000000004</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>0.6</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>0.65</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>0.7</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>0.75</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>0.8</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>0.85</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>0.9</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>0.95</v>
       </c>
@@ -2585,7 +2585,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
       <c r="C61" t="s">
         <v>7</v>
       </c>
@@ -2626,7 +2629,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.39741199999999999</v>
+      </c>
       <c r="C62">
         <v>0.1</v>
       </c>
@@ -2683,7 +2689,10 @@
         <v>600</v>
       </c>
     </row>
-    <row r="63" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0.116697</v>
+      </c>
       <c r="C63">
         <v>0.15</v>
       </c>
@@ -2740,7 +2749,10 @@
         <v>600</v>
       </c>
     </row>
-    <row r="64" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>7.8047000000000005E-2</v>
+      </c>
       <c r="C64">
         <v>0.2</v>
       </c>
@@ -2797,7 +2809,10 @@
         <v>600</v>
       </c>
     </row>
-    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.21759700000000001</v>
+      </c>
       <c r="C65">
         <v>0.25</v>
       </c>
@@ -2854,7 +2869,10 @@
         <v>600</v>
       </c>
     </row>
-    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.190248</v>
+      </c>
       <c r="C66">
         <v>0.3</v>
       </c>
@@ -2911,7 +2929,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>0.35</v>
       </c>
@@ -2968,7 +2986,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>0.4</v>
       </c>
@@ -3025,7 +3043,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="69" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>0.45</v>
       </c>
@@ -3082,7 +3100,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="70" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>0.5</v>
       </c>
@@ -3139,7 +3157,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="71" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>0.55000000000000004</v>
       </c>
@@ -3196,7 +3214,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="72" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>0.6</v>
       </c>
@@ -3253,7 +3271,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>0.65</v>
       </c>
@@ -3310,7 +3328,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="74" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>0.7</v>
       </c>
@@ -3367,7 +3385,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="75" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C75">
         <v>0.75</v>
       </c>
@@ -3424,7 +3442,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C76">
         <v>0.8</v>
       </c>
@@ -3481,7 +3499,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C77">
         <v>0.85</v>
       </c>
@@ -3538,7 +3556,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C78">
         <v>0.9</v>
       </c>
@@ -3595,7 +3613,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C79">
         <v>0.95</v>
       </c>
@@ -3652,7 +3670,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P80">
         <f>SUM(P62:P79)</f>
         <v>10800</v>

</xml_diff>